<commit_message>
update import and show detail
</commit_message>
<xml_diff>
--- a/public/excel/format_pbj/pbjana1.xlsx
+++ b/public/excel/format_pbj/pbjana1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\membership_laravel\public\excel\format_pbj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96E9D48-33C8-4DBB-85AC-6BE2877A2C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B680952-5E45-4693-BFC6-5031B8734FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="233">
   <si>
     <t>adimoo22@gmail.com</t>
   </si>
@@ -685,6 +685,48 @@
   </si>
   <si>
     <t>tempat_tanggal_lahir</t>
+  </si>
+  <si>
+    <t>nama_tanpa_gelar</t>
+  </si>
+  <si>
+    <t>Adi Purnomo</t>
+  </si>
+  <si>
+    <t>Ibrahim Novik</t>
+  </si>
+  <si>
+    <t>Witarya</t>
+  </si>
+  <si>
+    <t>WINDA AYUS PIKA</t>
+  </si>
+  <si>
+    <t>Nurwandi</t>
+  </si>
+  <si>
+    <t>Jhun</t>
+  </si>
+  <si>
+    <t>Syarifuddin</t>
+  </si>
+  <si>
+    <t>Nurfajri Mursalin</t>
+  </si>
+  <si>
+    <t>Cici Saputri</t>
+  </si>
+  <si>
+    <t>OKTOVINA WOPI</t>
+  </si>
+  <si>
+    <t>Welius Wetapo</t>
+  </si>
+  <si>
+    <t>Alexander Patandean</t>
+  </si>
+  <si>
+    <t>sulastri Litha</t>
   </si>
 </sst>
 </file>
@@ -1002,34 +1044,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB15"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="80.42578125" customWidth="1"/>
-    <col min="12" max="15" width="18.85546875" customWidth="1"/>
-    <col min="16" max="16" width="47.7109375" customWidth="1"/>
-    <col min="17" max="18" width="18.85546875" customWidth="1"/>
-    <col min="19" max="19" width="44.7109375" customWidth="1"/>
-    <col min="20" max="21" width="18.85546875" customWidth="1"/>
-    <col min="22" max="22" width="59.140625" customWidth="1"/>
-    <col min="23" max="28" width="18.85546875" customWidth="1"/>
+    <col min="2" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="80.42578125" customWidth="1"/>
+    <col min="13" max="16" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="47.7109375" customWidth="1"/>
+    <col min="18" max="19" width="18.85546875" customWidth="1"/>
+    <col min="20" max="20" width="44.7109375" customWidth="1"/>
+    <col min="21" max="22" width="18.85546875" customWidth="1"/>
+    <col min="23" max="23" width="59.140625" customWidth="1"/>
+    <col min="24" max="29" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>197</v>
       </c>
@@ -1037,1035 +1079,1077 @@
         <v>198</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>41361</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>91512</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>91512</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>91512</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="V5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>6709</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>12160</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="T6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="U6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="V6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="W6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>99358</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T7" s="5" t="s">
+      <c r="U7" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="V7" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="W7" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>91512</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="T8" s="5" t="s">
+      <c r="U8" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="V8" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="W8" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:28" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>90552</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="U9" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="U9" s="5" t="s">
+      <c r="V9" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="W9" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>99511</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="U10" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="U10" s="5" t="s">
+      <c r="V10" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="V10" s="5" t="s">
+      <c r="W10" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>99511</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="R11" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="T11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T11" s="5" t="s">
+      <c r="U11" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="U11" s="5" t="s">
+      <c r="V11" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="V11" s="5" t="s">
+      <c r="W11" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>99511</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="S12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T12" s="5" t="s">
+      <c r="U12" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="V12" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="V12" s="5" t="s">
+      <c r="W12" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>91811</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="R13" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="T13" s="5" t="s">
+      <c r="U13" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="V13" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="V13" s="5" t="s">
+      <c r="W13" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>91811</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="N14" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="R14" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="S14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="T14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="U14" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="V14" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="V14" s="5" t="s">
+      <c r="W14" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2094,48 +2178,49 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{5E48AC14-871C-4870-BEF3-04C4D544563E}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{BE75538D-E74F-45CD-864E-F9FF729FDE7C}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{5CB0CBC2-C941-4A45-9F91-BA35BF1E19B7}"/>
-    <hyperlink ref="T3" r:id="rId4" xr:uid="{ED3C63F7-7AC2-4065-8EE8-DECE886D20A6}"/>
-    <hyperlink ref="U3" r:id="rId5" xr:uid="{CAC924D1-2E65-456E-BBC2-9345CA37959B}"/>
-    <hyperlink ref="V3" r:id="rId6" xr:uid="{7AC5E653-CE1F-4810-A1A6-9F0D041D5F96}"/>
-    <hyperlink ref="T4" r:id="rId7" xr:uid="{38EFAC0B-3BBA-4048-8715-06EE0E557C9D}"/>
-    <hyperlink ref="U4" r:id="rId8" xr:uid="{3B1E0B56-95EA-4579-B569-3F4C439F0560}"/>
-    <hyperlink ref="V4" r:id="rId9" xr:uid="{30997B00-E2DE-4BC2-BC84-CE418EC2B994}"/>
-    <hyperlink ref="T5" r:id="rId10" xr:uid="{A1FD4005-8AE7-4901-8C15-0BF49D50649E}"/>
-    <hyperlink ref="U5" r:id="rId11" xr:uid="{3AA45C3C-B1A5-4594-AE7D-C503F283C02B}"/>
-    <hyperlink ref="V5" r:id="rId12" xr:uid="{45F11D64-68AE-4751-93E5-7A07EECED051}"/>
-    <hyperlink ref="T6" r:id="rId13" xr:uid="{F1CF6E76-2EE8-4DD7-8FF6-1F817703F0F3}"/>
-    <hyperlink ref="U6" r:id="rId14" xr:uid="{AB00F3E2-87DA-47B1-8A97-F213F232B513}"/>
-    <hyperlink ref="V6" r:id="rId15" xr:uid="{E9EE1F0B-E180-4B98-9060-8F59EF6D4877}"/>
-    <hyperlink ref="T7" r:id="rId16" xr:uid="{36A6E64E-1988-4154-BD38-0F560E601C74}"/>
-    <hyperlink ref="U7" r:id="rId17" xr:uid="{585EBA87-1B09-48CE-80D5-F6C4CF47AACA}"/>
-    <hyperlink ref="V7" r:id="rId18" xr:uid="{52B8B06D-AB5D-44B1-A942-045C49956441}"/>
-    <hyperlink ref="T8" r:id="rId19" xr:uid="{A7974C4D-D572-4A04-983F-B2885B9F94D2}"/>
-    <hyperlink ref="U8" r:id="rId20" xr:uid="{ABE931D5-F632-49BF-8013-A79B7FD624C9}"/>
-    <hyperlink ref="V8" r:id="rId21" xr:uid="{B00D0651-64D4-484B-8E6D-14C7F7719F08}"/>
-    <hyperlink ref="T9" r:id="rId22" xr:uid="{152D3E49-8855-4ABA-8E37-9A1FCE5AE213}"/>
-    <hyperlink ref="U9" r:id="rId23" xr:uid="{5F166103-A48A-4F86-B3F0-D0000A8DC39F}"/>
-    <hyperlink ref="V9" r:id="rId24" xr:uid="{1D0E985B-A604-43DD-8632-A61141DB441C}"/>
-    <hyperlink ref="T10" r:id="rId25" xr:uid="{1C0F8184-CAB8-4FD1-B801-48D07ADFBFA1}"/>
-    <hyperlink ref="U10" r:id="rId26" xr:uid="{B79D7D17-AE75-4DE7-BE9D-141B46A69465}"/>
-    <hyperlink ref="V10" r:id="rId27" xr:uid="{A8EEA2AE-1EAC-4EED-992B-132A3DA1386B}"/>
-    <hyperlink ref="T11" r:id="rId28" xr:uid="{88D903D9-7DD3-45F6-A5D0-98015840D2D6}"/>
-    <hyperlink ref="U11" r:id="rId29" xr:uid="{A2D2CF74-FF7A-4E03-81EC-6EE751F08D25}"/>
-    <hyperlink ref="V11" r:id="rId30" xr:uid="{4C52EAF4-23FC-4F99-934C-F4DB6D9025EB}"/>
-    <hyperlink ref="T12" r:id="rId31" xr:uid="{762217C0-31AF-4353-B81D-402C34CA30FC}"/>
-    <hyperlink ref="U12" r:id="rId32" xr:uid="{4A98B546-324A-4317-89A1-35CC24336018}"/>
-    <hyperlink ref="V12" r:id="rId33" xr:uid="{849A79C1-748A-4A9A-B376-4C1E8D2A7672}"/>
-    <hyperlink ref="T13" r:id="rId34" xr:uid="{93FB469C-3272-47BF-8259-69B035090559}"/>
-    <hyperlink ref="U13" r:id="rId35" xr:uid="{DD29A81F-1640-4657-89EB-F87514A0A253}"/>
-    <hyperlink ref="V13" r:id="rId36" xr:uid="{BA24FD39-4137-4363-86CA-EC373010223D}"/>
-    <hyperlink ref="T14" r:id="rId37" xr:uid="{6B7E762A-D780-41B4-9EF8-15187A91D2E0}"/>
-    <hyperlink ref="U14" r:id="rId38" xr:uid="{2A45983A-26CA-41C8-8E7D-85E51D372AD8}"/>
-    <hyperlink ref="V14" r:id="rId39" xr:uid="{554FE94B-C47F-466F-85F6-17144F0B7B97}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{5E48AC14-871C-4870-BEF3-04C4D544563E}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{BE75538D-E74F-45CD-864E-F9FF729FDE7C}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{5CB0CBC2-C941-4A45-9F91-BA35BF1E19B7}"/>
+    <hyperlink ref="U3" r:id="rId4" xr:uid="{ED3C63F7-7AC2-4065-8EE8-DECE886D20A6}"/>
+    <hyperlink ref="V3" r:id="rId5" xr:uid="{CAC924D1-2E65-456E-BBC2-9345CA37959B}"/>
+    <hyperlink ref="W3" r:id="rId6" xr:uid="{7AC5E653-CE1F-4810-A1A6-9F0D041D5F96}"/>
+    <hyperlink ref="U4" r:id="rId7" xr:uid="{38EFAC0B-3BBA-4048-8715-06EE0E557C9D}"/>
+    <hyperlink ref="V4" r:id="rId8" xr:uid="{3B1E0B56-95EA-4579-B569-3F4C439F0560}"/>
+    <hyperlink ref="W4" r:id="rId9" xr:uid="{30997B00-E2DE-4BC2-BC84-CE418EC2B994}"/>
+    <hyperlink ref="U5" r:id="rId10" xr:uid="{A1FD4005-8AE7-4901-8C15-0BF49D50649E}"/>
+    <hyperlink ref="V5" r:id="rId11" xr:uid="{3AA45C3C-B1A5-4594-AE7D-C503F283C02B}"/>
+    <hyperlink ref="W5" r:id="rId12" xr:uid="{45F11D64-68AE-4751-93E5-7A07EECED051}"/>
+    <hyperlink ref="U6" r:id="rId13" xr:uid="{F1CF6E76-2EE8-4DD7-8FF6-1F817703F0F3}"/>
+    <hyperlink ref="V6" r:id="rId14" xr:uid="{AB00F3E2-87DA-47B1-8A97-F213F232B513}"/>
+    <hyperlink ref="W6" r:id="rId15" xr:uid="{E9EE1F0B-E180-4B98-9060-8F59EF6D4877}"/>
+    <hyperlink ref="U7" r:id="rId16" xr:uid="{36A6E64E-1988-4154-BD38-0F560E601C74}"/>
+    <hyperlink ref="V7" r:id="rId17" xr:uid="{585EBA87-1B09-48CE-80D5-F6C4CF47AACA}"/>
+    <hyperlink ref="W7" r:id="rId18" xr:uid="{52B8B06D-AB5D-44B1-A942-045C49956441}"/>
+    <hyperlink ref="U8" r:id="rId19" xr:uid="{A7974C4D-D572-4A04-983F-B2885B9F94D2}"/>
+    <hyperlink ref="V8" r:id="rId20" xr:uid="{ABE931D5-F632-49BF-8013-A79B7FD624C9}"/>
+    <hyperlink ref="W8" r:id="rId21" xr:uid="{B00D0651-64D4-484B-8E6D-14C7F7719F08}"/>
+    <hyperlink ref="U9" r:id="rId22" xr:uid="{152D3E49-8855-4ABA-8E37-9A1FCE5AE213}"/>
+    <hyperlink ref="V9" r:id="rId23" xr:uid="{5F166103-A48A-4F86-B3F0-D0000A8DC39F}"/>
+    <hyperlink ref="W9" r:id="rId24" xr:uid="{1D0E985B-A604-43DD-8632-A61141DB441C}"/>
+    <hyperlink ref="U10" r:id="rId25" xr:uid="{1C0F8184-CAB8-4FD1-B801-48D07ADFBFA1}"/>
+    <hyperlink ref="V10" r:id="rId26" xr:uid="{B79D7D17-AE75-4DE7-BE9D-141B46A69465}"/>
+    <hyperlink ref="W10" r:id="rId27" xr:uid="{A8EEA2AE-1EAC-4EED-992B-132A3DA1386B}"/>
+    <hyperlink ref="U11" r:id="rId28" xr:uid="{88D903D9-7DD3-45F6-A5D0-98015840D2D6}"/>
+    <hyperlink ref="V11" r:id="rId29" xr:uid="{A2D2CF74-FF7A-4E03-81EC-6EE751F08D25}"/>
+    <hyperlink ref="W11" r:id="rId30" xr:uid="{4C52EAF4-23FC-4F99-934C-F4DB6D9025EB}"/>
+    <hyperlink ref="U12" r:id="rId31" xr:uid="{762217C0-31AF-4353-B81D-402C34CA30FC}"/>
+    <hyperlink ref="V12" r:id="rId32" xr:uid="{4A98B546-324A-4317-89A1-35CC24336018}"/>
+    <hyperlink ref="W12" r:id="rId33" xr:uid="{849A79C1-748A-4A9A-B376-4C1E8D2A7672}"/>
+    <hyperlink ref="U13" r:id="rId34" xr:uid="{93FB469C-3272-47BF-8259-69B035090559}"/>
+    <hyperlink ref="V13" r:id="rId35" xr:uid="{DD29A81F-1640-4657-89EB-F87514A0A253}"/>
+    <hyperlink ref="W13" r:id="rId36" xr:uid="{BA24FD39-4137-4363-86CA-EC373010223D}"/>
+    <hyperlink ref="U14" r:id="rId37" xr:uid="{6B7E762A-D780-41B4-9EF8-15187A91D2E0}"/>
+    <hyperlink ref="V14" r:id="rId38" xr:uid="{2A45983A-26CA-41C8-8E7D-85E51D372AD8}"/>
+    <hyperlink ref="W14" r:id="rId39" xr:uid="{554FE94B-C47F-466F-85F6-17144F0B7B97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>